<commit_message>
CANS-56. Domain item description and rating language refactored
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank_2018-06-17.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank_2018-06-17.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcordell\Documents\Documents\MHDATA Deliverables\CDSS\CANS\Final\Final4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metquota/cwds/cans-api/tools/instrument-parser/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A380582-46F7-4473-97C8-DE14B4DA5BC1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E6E9504D-FB31-014E-B29F-E40F95A91968}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9036" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="1980" windowWidth="29960" windowHeight="18320" tabRatio="555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="4" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Domain_Items" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Domain_Items!$A$1:$D$99</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$A$1:$V$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Domain_Items!$A$1:$D$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$A$1:$W$83</definedName>
     <definedName name="_Toc328064535" localSheetId="1">Items!$I$3</definedName>
     <definedName name="_Toc513575314" localSheetId="0">Domains!$B$4</definedName>
   </definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="779">
   <si>
     <t>Domain_ID</t>
   </si>
@@ -3075,9 +3075,6 @@
   </si>
   <si>
     <t>FAMILY_SPRITUAL_RELIGIOUS</t>
-  </si>
-  <si>
-    <t>CAREGIVER_EMOTIONAL RESPONSIVENESS</t>
   </si>
   <si>
     <t>CAREGIVER_ADJ_TRAUMA_EXP</t>
@@ -3125,6 +3122,18 @@
   </si>
   <si>
     <t>Background_Needs</t>
+  </si>
+  <si>
+    <t>Rate_NA</t>
+  </si>
+  <si>
+    <t>MEDICAL_PHYSICAL_CAREGIVER</t>
+  </si>
+  <si>
+    <t>SUBSTANCE_USE_CAREGIVER</t>
+  </si>
+  <si>
+    <t>CAREGIVER_EMOTIONAL_RESPONSIVENESS</t>
   </si>
 </sst>
 </file>
@@ -3159,12 +3168,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3188,7 +3203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3210,6 +3225,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3526,21 +3545,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="5"/>
+    <col min="6" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3584,7 +3603,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3619,7 +3638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3654,7 +3673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3689,7 +3708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3724,7 +3743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3759,7 +3778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3797,7 +3816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3829,7 +3848,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3858,7 +3877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3887,7 +3906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3916,7 +3935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3945,7 +3964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3974,7 +3993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -4010,35 +4029,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V83"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="255.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.5" style="2" customWidth="1"/>
     <col min="7" max="12" width="7.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="93.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="7.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="7.6640625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="93.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="7.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>410</v>
       </c>
@@ -4075,38 +4095,41 @@
       <c r="L1" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>775</v>
-      </c>
       <c r="T1" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4134,20 +4157,20 @@
       <c r="J2" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4178,23 +4201,23 @@
       <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="2">
         <v>1</v>
       </c>
-      <c r="T3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4225,23 +4248,23 @@
       <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
       <c r="P4" s="2">
         <v>1</v>
       </c>
       <c r="Q4" s="2">
         <v>1</v>
       </c>
-      <c r="T4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4272,23 +4295,23 @@
       <c r="J5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
       <c r="P5" s="2">
         <v>1</v>
       </c>
       <c r="Q5" s="2">
         <v>1</v>
       </c>
-      <c r="T5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4319,23 +4342,23 @@
       <c r="J6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="2">
-        <v>1</v>
-      </c>
       <c r="P6" s="2">
         <v>1</v>
       </c>
       <c r="Q6" s="2">
         <v>1</v>
       </c>
-      <c r="T6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4363,20 +4386,20 @@
       <c r="J7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
       <c r="Q7" s="2">
         <v>1</v>
       </c>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4404,23 +4427,23 @@
       <c r="J8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="P8" s="2">
-        <v>1</v>
-      </c>
       <c r="Q8" s="2">
         <v>1</v>
       </c>
-      <c r="T8" s="2">
+      <c r="R8" s="2">
         <v>1</v>
       </c>
       <c r="U8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4448,20 +4471,20 @@
       <c r="J9" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="2">
-        <v>1</v>
-      </c>
       <c r="Q9" s="2">
         <v>1</v>
       </c>
-      <c r="T9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="2">
+        <v>1</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4492,23 +4515,23 @@
       <c r="J10" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
       <c r="P10" s="2">
         <v>1</v>
       </c>
       <c r="Q10" s="2">
         <v>1</v>
       </c>
-      <c r="T10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4522,7 +4545,7 @@
         <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>414</v>
@@ -4539,23 +4562,23 @@
       <c r="J11" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="O11" s="2">
-        <v>1</v>
-      </c>
       <c r="P11" s="2">
         <v>1</v>
       </c>
       <c r="Q11" s="2">
         <v>1</v>
       </c>
-      <c r="T11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+      <c r="U11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -4583,20 +4606,20 @@
       <c r="J12" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="P12" s="2">
-        <v>1</v>
-      </c>
       <c r="Q12" s="2">
         <v>1</v>
       </c>
-      <c r="T12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+      <c r="U12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -4624,20 +4647,20 @@
       <c r="J13" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="P13" s="2">
-        <v>1</v>
-      </c>
       <c r="Q13" s="2">
         <v>1</v>
       </c>
-      <c r="T13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
+      <c r="U13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -4668,23 +4691,23 @@
       <c r="J14" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="O14" s="2">
-        <v>1</v>
-      </c>
       <c r="P14" s="2">
         <v>1</v>
       </c>
       <c r="Q14" s="2">
         <v>1</v>
       </c>
-      <c r="T14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4712,20 +4735,20 @@
       <c r="J15" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="P15" s="2">
-        <v>1</v>
-      </c>
       <c r="Q15" s="2">
         <v>1</v>
       </c>
-      <c r="T15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R15" s="2">
+        <v>1</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4753,20 +4776,20 @@
       <c r="J16" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
       <c r="Q16" s="2">
         <v>1</v>
       </c>
-      <c r="T16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R16" s="2">
+        <v>1</v>
+      </c>
+      <c r="U16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4794,20 +4817,20 @@
       <c r="J17" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="P17" s="2">
-        <v>1</v>
-      </c>
       <c r="Q17" s="2">
         <v>1</v>
       </c>
-      <c r="T17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+      <c r="U17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -4835,20 +4858,20 @@
       <c r="J18" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="P18" s="2">
-        <v>1</v>
-      </c>
       <c r="Q18" s="2">
         <v>1</v>
       </c>
-      <c r="T18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4879,20 +4902,20 @@
       <c r="J19" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="P19" s="2">
-        <v>1</v>
-      </c>
       <c r="Q19" s="2">
         <v>1</v>
       </c>
-      <c r="T19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+      <c r="U19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4920,20 +4943,20 @@
       <c r="J20" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="P20" s="2">
-        <v>1</v>
-      </c>
       <c r="Q20" s="2">
         <v>1</v>
       </c>
-      <c r="T20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+      <c r="U20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4964,23 +4987,26 @@
       <c r="J21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="9">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="O21" s="2">
-        <v>1</v>
-      </c>
       <c r="P21" s="2">
         <v>1</v>
       </c>
       <c r="Q21" s="2">
         <v>1</v>
       </c>
-      <c r="T21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -5008,23 +5034,23 @@
       <c r="J22" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="P22" s="2">
-        <v>1</v>
-      </c>
       <c r="Q22" s="2">
         <v>1</v>
       </c>
-      <c r="T22" s="2">
+      <c r="R22" s="2">
         <v>1</v>
       </c>
       <c r="U22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -5052,23 +5078,23 @@
       <c r="J23" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="N23" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="P23" s="2">
-        <v>1</v>
-      </c>
       <c r="Q23" s="2">
         <v>1</v>
       </c>
-      <c r="T23" s="2">
+      <c r="R23" s="2">
         <v>1</v>
       </c>
       <c r="U23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -5096,23 +5122,23 @@
       <c r="J24" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="P24" s="2">
-        <v>1</v>
-      </c>
       <c r="Q24" s="2">
         <v>1</v>
       </c>
-      <c r="T24" s="2">
+      <c r="R24" s="2">
         <v>1</v>
       </c>
       <c r="U24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -5140,23 +5166,23 @@
       <c r="J25" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="N25" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="P25" s="2">
-        <v>1</v>
-      </c>
       <c r="Q25" s="2">
         <v>1</v>
       </c>
-      <c r="T25" s="2">
-        <v>1</v>
-      </c>
-      <c r="V25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R25" s="2">
+        <v>1</v>
+      </c>
+      <c r="U25" s="2">
+        <v>1</v>
+      </c>
+      <c r="W25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -5184,23 +5210,23 @@
       <c r="J26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="P26" s="2">
-        <v>1</v>
-      </c>
       <c r="Q26" s="2">
         <v>1</v>
       </c>
-      <c r="T26" s="2">
+      <c r="R26" s="2">
         <v>1</v>
       </c>
       <c r="U26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -5228,23 +5254,23 @@
       <c r="J27" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="P27" s="2">
-        <v>1</v>
-      </c>
       <c r="Q27" s="2">
         <v>1</v>
       </c>
-      <c r="T27" s="2">
-        <v>1</v>
-      </c>
-      <c r="V27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R27" s="2">
+        <v>1</v>
+      </c>
+      <c r="U27" s="2">
+        <v>1</v>
+      </c>
+      <c r="W27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -5272,16 +5298,13 @@
       <c r="J28" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="P28" s="2">
-        <v>1</v>
-      </c>
       <c r="Q28" s="2">
         <v>1</v>
       </c>
-      <c r="T28" s="2">
+      <c r="R28" s="2">
         <v>1</v>
       </c>
       <c r="U28" s="2">
@@ -5290,8 +5313,11 @@
       <c r="V28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5319,20 +5345,20 @@
       <c r="J29" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="P29" s="2">
-        <v>1</v>
-      </c>
       <c r="Q29" s="2">
         <v>1</v>
       </c>
-      <c r="T29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R29" s="2">
+        <v>1</v>
+      </c>
+      <c r="U29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5363,23 +5389,23 @@
       <c r="J30" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="O30" s="2">
-        <v>1</v>
-      </c>
       <c r="P30" s="2">
         <v>1</v>
       </c>
       <c r="Q30" s="2">
         <v>1</v>
       </c>
-      <c r="T30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="2">
+        <v>1</v>
+      </c>
+      <c r="U30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5410,23 +5436,23 @@
       <c r="J31" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="O31" s="2">
-        <v>1</v>
-      </c>
       <c r="P31" s="2">
         <v>1</v>
       </c>
       <c r="Q31" s="2">
         <v>1</v>
       </c>
-      <c r="T31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R31" s="2">
+        <v>1</v>
+      </c>
+      <c r="U31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5457,23 +5483,23 @@
       <c r="J32" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="O32" s="2">
-        <v>1</v>
-      </c>
       <c r="P32" s="2">
         <v>1</v>
       </c>
       <c r="Q32" s="2">
         <v>1</v>
       </c>
-      <c r="T32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="2">
+        <v>1</v>
+      </c>
+      <c r="U32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5504,23 +5530,23 @@
       <c r="J33" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="O33" s="2">
-        <v>1</v>
-      </c>
       <c r="P33" s="2">
         <v>1</v>
       </c>
-      <c r="R33" s="2">
-        <v>1</v>
-      </c>
-      <c r="T33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q33" s="2">
+        <v>1</v>
+      </c>
+      <c r="S33" s="2">
+        <v>1</v>
+      </c>
+      <c r="U33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5551,26 +5577,26 @@
       <c r="J34" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="O34" s="2">
-        <v>1</v>
-      </c>
       <c r="P34" s="2">
         <v>1</v>
       </c>
-      <c r="R34" s="2">
-        <v>1</v>
-      </c>
-      <c r="T34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q34" s="2">
+        <v>1</v>
+      </c>
+      <c r="S34" s="2">
+        <v>1</v>
+      </c>
+      <c r="U34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5598,20 +5624,23 @@
       <c r="J35" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="9">
+        <v>1</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="P35" s="2">
-        <v>1</v>
-      </c>
-      <c r="R35" s="2">
-        <v>1</v>
-      </c>
-      <c r="T35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="2">
+        <v>1</v>
+      </c>
+      <c r="S35" s="2">
+        <v>1</v>
+      </c>
+      <c r="U35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5639,20 +5668,20 @@
       <c r="J36" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="P36" s="2">
-        <v>1</v>
-      </c>
-      <c r="R36" s="2">
-        <v>1</v>
-      </c>
-      <c r="T36" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="2">
+        <v>1</v>
+      </c>
+      <c r="S36" s="2">
+        <v>1</v>
+      </c>
+      <c r="U36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5680,20 +5709,20 @@
       <c r="J37" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="N37" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="P37" s="2">
-        <v>1</v>
-      </c>
-      <c r="R37" s="2">
-        <v>1</v>
-      </c>
-      <c r="T37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q37" s="2">
+        <v>1</v>
+      </c>
+      <c r="S37" s="2">
+        <v>1</v>
+      </c>
+      <c r="U37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5721,20 +5750,20 @@
       <c r="J38" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="N38" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="P38" s="2">
-        <v>1</v>
-      </c>
-      <c r="R38" s="2">
-        <v>1</v>
-      </c>
-      <c r="T38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q38" s="2">
+        <v>1</v>
+      </c>
+      <c r="S38" s="2">
+        <v>1</v>
+      </c>
+      <c r="U38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5762,20 +5791,20 @@
       <c r="J39" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="P39" s="2">
-        <v>1</v>
-      </c>
-      <c r="R39" s="2">
-        <v>1</v>
-      </c>
-      <c r="T39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q39" s="2">
+        <v>1</v>
+      </c>
+      <c r="S39" s="2">
+        <v>1</v>
+      </c>
+      <c r="U39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5806,20 +5835,20 @@
       <c r="J40" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="P40" s="2">
-        <v>1</v>
-      </c>
-      <c r="R40" s="2">
-        <v>1</v>
-      </c>
-      <c r="T40" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q40" s="2">
+        <v>1</v>
+      </c>
+      <c r="S40" s="2">
+        <v>1</v>
+      </c>
+      <c r="U40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5850,23 +5879,23 @@
       <c r="J41" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="O41" s="2">
-        <v>1</v>
-      </c>
       <c r="P41" s="2">
         <v>1</v>
       </c>
-      <c r="R41" s="2">
-        <v>1</v>
-      </c>
-      <c r="T41" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q41" s="2">
+        <v>1</v>
+      </c>
+      <c r="S41" s="2">
+        <v>1</v>
+      </c>
+      <c r="U41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -5897,23 +5926,23 @@
       <c r="J42" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="O42" s="2">
-        <v>1</v>
-      </c>
       <c r="P42" s="2">
         <v>1</v>
       </c>
       <c r="Q42" s="2">
         <v>1</v>
       </c>
-      <c r="T42" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R42" s="2">
+        <v>1</v>
+      </c>
+      <c r="U42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5944,23 +5973,23 @@
       <c r="J43" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="M43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="O43" s="2">
-        <v>1</v>
-      </c>
       <c r="P43" s="2">
         <v>1</v>
       </c>
       <c r="Q43" s="2">
         <v>1</v>
       </c>
-      <c r="T43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R43" s="2">
+        <v>1</v>
+      </c>
+      <c r="U43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -5991,26 +6020,26 @@
       <c r="J44" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="M44" s="2" t="s">
+      <c r="N44" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="O44" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="O44" s="2">
-        <v>1</v>
-      </c>
       <c r="P44" s="2">
         <v>1</v>
       </c>
       <c r="Q44" s="2">
         <v>1</v>
       </c>
-      <c r="T44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R44" s="2">
+        <v>1</v>
+      </c>
+      <c r="U44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -6041,23 +6070,23 @@
       <c r="J45" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="O45" s="2">
-        <v>1</v>
-      </c>
       <c r="P45" s="2">
         <v>1</v>
       </c>
       <c r="Q45" s="2">
         <v>1</v>
       </c>
-      <c r="T45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="2">
+        <v>1</v>
+      </c>
+      <c r="U45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -6074,7 +6103,7 @@
         <v>731</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>590</v>
@@ -6088,23 +6117,23 @@
       <c r="J46" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="O46" s="2">
-        <v>1</v>
-      </c>
       <c r="P46" s="2">
         <v>1</v>
       </c>
       <c r="Q46" s="2">
         <v>1</v>
       </c>
-      <c r="T46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R46" s="2">
+        <v>1</v>
+      </c>
+      <c r="U46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -6117,8 +6146,8 @@
       <c r="D47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>732</v>
+      <c r="E47" s="9" t="s">
+        <v>776</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>594</v>
@@ -6135,23 +6164,23 @@
       <c r="J47" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="O47" s="2">
-        <v>1</v>
-      </c>
       <c r="P47" s="2">
         <v>1</v>
       </c>
       <c r="Q47" s="2">
         <v>1</v>
       </c>
-      <c r="T47" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R47" s="2">
+        <v>1</v>
+      </c>
+      <c r="U47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -6182,23 +6211,23 @@
       <c r="J48" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="O48" s="2">
-        <v>1</v>
-      </c>
       <c r="P48" s="2">
         <v>1</v>
       </c>
       <c r="Q48" s="2">
         <v>1</v>
       </c>
-      <c r="T48" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R48" s="2">
+        <v>1</v>
+      </c>
+      <c r="U48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -6211,8 +6240,8 @@
       <c r="D49" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>714</v>
+      <c r="E49" s="9" t="s">
+        <v>777</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>137</v>
@@ -6229,26 +6258,26 @@
       <c r="J49" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="O49" s="2">
-        <v>1</v>
-      </c>
       <c r="P49" s="2">
         <v>1</v>
       </c>
       <c r="Q49" s="2">
         <v>1</v>
       </c>
-      <c r="T49" s="2">
+      <c r="R49" s="2">
         <v>1</v>
       </c>
       <c r="U49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -6279,23 +6308,23 @@
       <c r="J50" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="M50" s="2" t="s">
+      <c r="N50" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="O50" s="2">
-        <v>1</v>
-      </c>
       <c r="P50" s="2">
         <v>1</v>
       </c>
       <c r="Q50" s="2">
         <v>1</v>
       </c>
-      <c r="T50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R50" s="2">
+        <v>1</v>
+      </c>
+      <c r="U50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -6326,23 +6355,23 @@
       <c r="J51" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="N51" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="O51" s="2">
-        <v>1</v>
-      </c>
       <c r="P51" s="2">
         <v>1</v>
       </c>
       <c r="Q51" s="2">
         <v>1</v>
       </c>
-      <c r="T51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R51" s="2">
+        <v>1</v>
+      </c>
+      <c r="U51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -6367,23 +6396,23 @@
       <c r="L52" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="M52" s="2" t="s">
+      <c r="N52" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="O52" s="2">
-        <v>1</v>
-      </c>
       <c r="P52" s="2">
         <v>1</v>
       </c>
       <c r="Q52" s="2">
         <v>1</v>
       </c>
-      <c r="S52" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R52" s="2">
+        <v>1</v>
+      </c>
+      <c r="T52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -6408,23 +6437,23 @@
       <c r="L53" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="M53" s="2" t="s">
+      <c r="N53" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="O53" s="2">
-        <v>1</v>
-      </c>
       <c r="P53" s="2">
         <v>1</v>
       </c>
       <c r="Q53" s="2">
         <v>1</v>
       </c>
-      <c r="S53" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R53" s="2">
+        <v>1</v>
+      </c>
+      <c r="T53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -6449,23 +6478,23 @@
       <c r="L54" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="M54" s="2" t="s">
+      <c r="N54" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="O54" s="2">
-        <v>1</v>
-      </c>
       <c r="P54" s="2">
         <v>1</v>
       </c>
       <c r="Q54" s="2">
         <v>1</v>
       </c>
-      <c r="S54" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R54" s="2">
+        <v>1</v>
+      </c>
+      <c r="T54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -6490,23 +6519,23 @@
       <c r="L55" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="N55" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="O55" s="2">
-        <v>1</v>
-      </c>
       <c r="P55" s="2">
         <v>1</v>
       </c>
       <c r="Q55" s="2">
         <v>1</v>
       </c>
-      <c r="S55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R55" s="2">
+        <v>1</v>
+      </c>
+      <c r="T55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -6531,26 +6560,26 @@
       <c r="L56" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="N56" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="N56" s="2" t="s">
+      <c r="O56" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="O56" s="2">
-        <v>1</v>
-      </c>
       <c r="P56" s="2">
         <v>1</v>
       </c>
       <c r="Q56" s="2">
         <v>1</v>
       </c>
-      <c r="S56" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R56" s="2">
+        <v>1</v>
+      </c>
+      <c r="T56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -6575,23 +6604,23 @@
       <c r="L57" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="N57" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="O57" s="2">
-        <v>1</v>
-      </c>
       <c r="P57" s="2">
         <v>1</v>
       </c>
       <c r="Q57" s="2">
         <v>1</v>
       </c>
-      <c r="S57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R57" s="2">
+        <v>1</v>
+      </c>
+      <c r="T57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -6616,23 +6645,23 @@
       <c r="L58" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="N58" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="O58" s="2">
-        <v>1</v>
-      </c>
       <c r="P58" s="2">
         <v>1</v>
       </c>
       <c r="Q58" s="2">
         <v>1</v>
       </c>
-      <c r="S58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R58" s="2">
+        <v>1</v>
+      </c>
+      <c r="T58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -6657,23 +6686,23 @@
       <c r="L59" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M59" s="2" t="s">
+      <c r="N59" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="O59" s="2">
-        <v>1</v>
-      </c>
       <c r="P59" s="2">
         <v>1</v>
       </c>
       <c r="Q59" s="2">
         <v>1</v>
       </c>
-      <c r="S59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R59" s="2">
+        <v>1</v>
+      </c>
+      <c r="T59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -6698,26 +6727,26 @@
       <c r="L60" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="N60" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="N60" s="2" t="s">
+      <c r="O60" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="O60" s="2">
-        <v>1</v>
-      </c>
       <c r="P60" s="2">
         <v>1</v>
       </c>
       <c r="Q60" s="2">
         <v>1</v>
       </c>
-      <c r="S60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R60" s="2">
+        <v>1</v>
+      </c>
+      <c r="T60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -6742,26 +6771,26 @@
       <c r="L61" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="M61" s="2" t="s">
+      <c r="N61" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="N61" s="2" t="s">
+      <c r="O61" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="O61" s="2">
-        <v>1</v>
-      </c>
       <c r="P61" s="2">
         <v>1</v>
       </c>
       <c r="Q61" s="2">
         <v>1</v>
       </c>
-      <c r="S61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R61" s="2">
+        <v>1</v>
+      </c>
+      <c r="T61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -6772,10 +6801,10 @@
         <v>187</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>188</v>
@@ -6786,26 +6815,26 @@
       <c r="L62" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="M62" s="2" t="s">
+      <c r="N62" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="N62" s="2" t="s">
+      <c r="O62" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="O62" s="2">
-        <v>1</v>
-      </c>
       <c r="P62" s="2">
         <v>1</v>
       </c>
       <c r="Q62" s="2">
         <v>1</v>
       </c>
-      <c r="S62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R62" s="2">
+        <v>1</v>
+      </c>
+      <c r="T62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -6830,23 +6859,23 @@
       <c r="L63" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="M63" s="2" t="s">
+      <c r="N63" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="O63" s="2">
-        <v>1</v>
-      </c>
       <c r="P63" s="2">
         <v>1</v>
       </c>
       <c r="Q63" s="2">
         <v>1</v>
       </c>
-      <c r="S63" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R63" s="2">
+        <v>1</v>
+      </c>
+      <c r="T63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -6874,23 +6903,23 @@
       <c r="J64" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="M64" s="2" t="s">
+      <c r="N64" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="O64" s="2">
-        <v>1</v>
-      </c>
-      <c r="P64" s="2" t="s">
+      <c r="P64" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q64" s="2">
-        <v>1</v>
-      </c>
-      <c r="T64" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R64" s="2">
+        <v>1</v>
+      </c>
+      <c r="U64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -6918,23 +6947,23 @@
       <c r="J65" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="M65" s="2" t="s">
+      <c r="N65" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="O65" s="2">
-        <v>1</v>
-      </c>
-      <c r="P65" s="2" t="s">
+      <c r="P65" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q65" s="2">
-        <v>1</v>
-      </c>
-      <c r="T65" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R65" s="2">
+        <v>1</v>
+      </c>
+      <c r="U65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -6962,23 +6991,23 @@
       <c r="J66" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="M66" s="2" t="s">
+      <c r="N66" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="O66" s="2">
-        <v>1</v>
-      </c>
-      <c r="P66" s="2" t="s">
+      <c r="P66" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q66" s="2">
-        <v>1</v>
-      </c>
-      <c r="T66" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R66" s="2">
+        <v>1</v>
+      </c>
+      <c r="U66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -7006,23 +7035,23 @@
       <c r="J67" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="M67" s="2" t="s">
+      <c r="N67" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="O67" s="2">
-        <v>1</v>
-      </c>
-      <c r="P67" s="2" t="s">
+      <c r="P67" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q67" s="2">
-        <v>1</v>
-      </c>
-      <c r="T67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R67" s="2">
+        <v>1</v>
+      </c>
+      <c r="U67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -7050,23 +7079,23 @@
       <c r="J68" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="M68" s="2" t="s">
+      <c r="N68" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="O68" s="2">
-        <v>1</v>
-      </c>
-      <c r="P68" s="2" t="s">
+      <c r="P68" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q68" s="2">
-        <v>1</v>
-      </c>
-      <c r="T68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R68" s="2">
+        <v>1</v>
+      </c>
+      <c r="U68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -7094,26 +7123,26 @@
       <c r="J69" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="M69" s="2" t="s">
+      <c r="N69" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="O69" s="2">
-        <v>1</v>
-      </c>
-      <c r="P69" s="2" t="s">
+      <c r="P69" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q69" s="2">
-        <v>1</v>
-      </c>
-      <c r="S69" s="2">
+      <c r="R69" s="2">
         <v>1</v>
       </c>
       <c r="T69" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -7141,26 +7170,26 @@
       <c r="J70" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="M70" s="2" t="s">
+      <c r="N70" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O70" s="2">
-        <v>1</v>
-      </c>
-      <c r="P70" s="2" t="s">
+      <c r="P70" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q70" s="2">
-        <v>1</v>
-      </c>
-      <c r="S70" s="2">
+      <c r="R70" s="2">
         <v>1</v>
       </c>
       <c r="T70" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -7188,26 +7217,26 @@
       <c r="J71" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="M71" s="2" t="s">
+      <c r="N71" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="O71" s="2">
-        <v>1</v>
-      </c>
-      <c r="P71" s="2" t="s">
+      <c r="P71" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q71" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q71" s="2">
-        <v>1</v>
-      </c>
-      <c r="S71" s="2">
+      <c r="R71" s="2">
         <v>1</v>
       </c>
       <c r="T71" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -7235,26 +7264,26 @@
       <c r="J72" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="M72" s="2" t="s">
+      <c r="N72" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="O72" s="2">
-        <v>1</v>
-      </c>
-      <c r="P72" s="2" t="s">
+      <c r="P72" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q72" s="2">
-        <v>1</v>
-      </c>
-      <c r="S72" s="2">
+      <c r="R72" s="2">
         <v>1</v>
       </c>
       <c r="T72" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -7282,26 +7311,26 @@
       <c r="J73" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="M73" s="2" t="s">
+      <c r="N73" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="O73" s="2">
-        <v>1</v>
-      </c>
-      <c r="P73" s="2" t="s">
+      <c r="P73" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q73" s="2">
-        <v>1</v>
-      </c>
-      <c r="S73" s="2">
+      <c r="R73" s="2">
         <v>1</v>
       </c>
       <c r="T73" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -7329,26 +7358,26 @@
       <c r="J74" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="M74" s="2" t="s">
+      <c r="N74" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="O74" s="2">
-        <v>1</v>
-      </c>
-      <c r="P74" s="2" t="s">
+      <c r="P74" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q74" s="2">
-        <v>1</v>
-      </c>
-      <c r="S74" s="2">
+      <c r="R74" s="2">
         <v>1</v>
       </c>
       <c r="T74" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -7376,26 +7405,26 @@
       <c r="J75" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="M75" s="2" t="s">
+      <c r="N75" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="O75" s="2">
-        <v>1</v>
-      </c>
-      <c r="P75" s="2" t="s">
+      <c r="P75" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q75" s="2">
-        <v>1</v>
-      </c>
-      <c r="S75" s="2">
+      <c r="R75" s="2">
         <v>1</v>
       </c>
       <c r="T75" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -7423,23 +7452,23 @@
       <c r="J76" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M76" s="2" t="s">
+      <c r="N76" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="O76" s="2">
-        <v>1</v>
-      </c>
-      <c r="P76" s="2" t="s">
+      <c r="P76" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q76" s="2">
-        <v>1</v>
-      </c>
-      <c r="T76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R76" s="2">
+        <v>1</v>
+      </c>
+      <c r="U76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -7449,8 +7478,8 @@
       <c r="D77" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>767</v>
+      <c r="E77" s="9" t="s">
+        <v>778</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>278</v>
@@ -7467,23 +7496,23 @@
       <c r="J77" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="M77" s="2" t="s">
+      <c r="N77" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="O77" s="2">
-        <v>1</v>
-      </c>
-      <c r="P77" s="2" t="s">
+      <c r="P77" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q77" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q77" s="2">
-        <v>1</v>
-      </c>
-      <c r="T77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R77" s="2">
+        <v>1</v>
+      </c>
+      <c r="U77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -7494,7 +7523,7 @@
         <v>285</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>286</v>
@@ -7511,23 +7540,23 @@
       <c r="J78" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="N78" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="O78" s="2">
-        <v>1</v>
-      </c>
-      <c r="P78" s="2" t="s">
+      <c r="P78" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q78" s="2">
-        <v>1</v>
-      </c>
-      <c r="T78" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R78" s="2">
+        <v>1</v>
+      </c>
+      <c r="U78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -7538,7 +7567,7 @@
         <v>292</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>293</v>
@@ -7555,23 +7584,23 @@
       <c r="J79" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="M79" s="2" t="s">
+      <c r="N79" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="O79" s="2">
-        <v>1</v>
-      </c>
-      <c r="P79" s="2" t="s">
+      <c r="P79" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q79" s="2">
-        <v>1</v>
-      </c>
-      <c r="T79" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R79" s="2">
+        <v>1</v>
+      </c>
+      <c r="U79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -7599,23 +7628,23 @@
       <c r="J80" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="N80" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="O80" s="2">
-        <v>1</v>
-      </c>
-      <c r="P80" s="2" t="s">
+      <c r="P80" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q80" s="2">
-        <v>1</v>
-      </c>
-      <c r="T80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R80" s="2">
+        <v>1</v>
+      </c>
+      <c r="U80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -7643,23 +7672,23 @@
       <c r="J81" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="O81" s="2">
-        <v>1</v>
-      </c>
-      <c r="P81" s="2" t="s">
+      <c r="P81" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q81" s="2">
-        <v>1</v>
-      </c>
-      <c r="T81" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R81" s="2">
+        <v>1</v>
+      </c>
+      <c r="U81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -7687,23 +7716,26 @@
       <c r="J82" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="M82" s="2" t="s">
+      <c r="M82" s="9">
+        <v>1</v>
+      </c>
+      <c r="N82" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="O82" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q82" s="2">
-        <v>1</v>
-      </c>
-      <c r="T82" s="2">
+      <c r="P82" s="2">
+        <v>1</v>
+      </c>
+      <c r="R82" s="2">
         <v>1</v>
       </c>
       <c r="U82" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -7731,23 +7763,23 @@
       <c r="J83" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="M83" s="2" t="s">
+      <c r="N83" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="Q83" s="2">
-        <v>1</v>
-      </c>
-      <c r="T83" s="2">
+      <c r="R83" s="2">
+        <v>1</v>
+      </c>
+      <c r="U83" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V83" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState ref="A2:V83">
+  <autoFilter ref="A1:W83" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState ref="A2:W83">
       <sortCondition ref="A1:A83"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A1:V91">
+  <sortState ref="A1:W91">
     <sortCondition ref="C2:C81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7759,19 +7791,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.109375" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.1640625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7785,7 +7817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7796,7 +7828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7807,7 +7839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -7818,7 +7850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -7829,7 +7861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -7840,7 +7872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -7851,7 +7883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -7862,7 +7894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -7873,7 +7905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -7884,7 +7916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -7895,7 +7927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -7906,7 +7938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>2</v>
       </c>
@@ -7917,7 +7949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>2</v>
       </c>
@@ -7928,7 +7960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -7939,7 +7971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -7950,7 +7982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>2</v>
       </c>
@@ -7961,7 +7993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>2</v>
       </c>
@@ -7972,7 +8004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>2</v>
       </c>
@@ -7983,7 +8015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>2</v>
       </c>
@@ -7994,7 +8026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -8005,7 +8037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>3</v>
       </c>
@@ -8016,7 +8048,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>3</v>
       </c>
@@ -8027,7 +8059,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>3</v>
       </c>
@@ -8038,7 +8070,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>3</v>
       </c>
@@ -8049,7 +8081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>3</v>
       </c>
@@ -8060,7 +8092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>3</v>
       </c>
@@ -8071,7 +8103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>3</v>
       </c>
@@ -8082,7 +8114,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>3</v>
       </c>
@@ -8093,7 +8125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>4</v>
       </c>
@@ -8104,7 +8136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>4</v>
       </c>
@@ -8115,7 +8147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>4</v>
       </c>
@@ -8126,7 +8158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>5</v>
       </c>
@@ -8137,7 +8169,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>5</v>
       </c>
@@ -8148,7 +8180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>5</v>
       </c>
@@ -8159,7 +8191,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>5</v>
       </c>
@@ -8170,7 +8202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>5</v>
       </c>
@@ -8181,7 +8213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>5</v>
       </c>
@@ -8192,7 +8224,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>5</v>
       </c>
@@ -8203,7 +8235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>5</v>
       </c>
@@ -8214,7 +8246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>5</v>
       </c>
@@ -8225,718 +8257,718 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
+        <v>8</v>
+      </c>
+      <c r="B42" s="5">
+        <v>2</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>8</v>
+      </c>
+      <c r="B43" s="5">
+        <v>3</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>8</v>
+      </c>
+      <c r="B44" s="5">
+        <v>4</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>8</v>
+      </c>
+      <c r="B45" s="5">
+        <v>5</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>8</v>
+      </c>
+      <c r="B46" s="5">
+        <v>9</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>8</v>
+      </c>
+      <c r="B47" s="5">
+        <v>20</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>8</v>
+      </c>
+      <c r="B48" s="5">
+        <v>63</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>8</v>
+      </c>
+      <c r="B49" s="5">
+        <v>64</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>8</v>
+      </c>
+      <c r="B50" s="5">
+        <v>65</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>9</v>
+      </c>
+      <c r="B51" s="5">
+        <v>10</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>9</v>
+      </c>
+      <c r="B52" s="5">
+        <v>13</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>9</v>
+      </c>
+      <c r="B53" s="5">
+        <v>18</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>9</v>
+      </c>
+      <c r="B54" s="5">
+        <v>66</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>10</v>
+      </c>
+      <c r="B55" s="5">
+        <v>67</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>10</v>
+      </c>
+      <c r="B56" s="5">
+        <v>68</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>10</v>
+      </c>
+      <c r="B57" s="5">
+        <v>69</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>10</v>
+      </c>
+      <c r="B58" s="5">
+        <v>70</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>10</v>
+      </c>
+      <c r="B59" s="5">
+        <v>71</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>10</v>
+      </c>
+      <c r="B60" s="5">
+        <v>72</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>10</v>
+      </c>
+      <c r="B61" s="5">
+        <v>81</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>11</v>
+      </c>
+      <c r="B62" s="5">
+        <v>29</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
+        <v>11</v>
+      </c>
+      <c r="B63" s="5">
+        <v>30</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>11</v>
+      </c>
+      <c r="B64" s="5">
+        <v>31</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>12</v>
+      </c>
+      <c r="B65" s="5">
+        <v>32</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>12</v>
+      </c>
+      <c r="B66" s="5">
+        <v>33</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>12</v>
+      </c>
+      <c r="B67" s="5">
+        <v>39</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>12</v>
+      </c>
+      <c r="B68" s="5">
+        <v>40</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>12</v>
+      </c>
+      <c r="B69" s="5">
+        <v>73</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>12</v>
+      </c>
+      <c r="B70" s="5">
+        <v>74</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>12</v>
+      </c>
+      <c r="B71" s="5">
+        <v>75</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>12</v>
+      </c>
+      <c r="B72" s="5">
+        <v>82</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
+        <v>13</v>
+      </c>
+      <c r="B73" s="5">
+        <v>76</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>13</v>
+      </c>
+      <c r="B74" s="5">
+        <v>77</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="10">
         <v>6</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B75" s="10">
         <v>41</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C75" s="10">
         <v>41</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D75" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+    <row r="76" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="10">
         <v>6</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B76" s="10">
         <v>42</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C76" s="10">
         <v>42</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D76" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+    <row r="77" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="10">
         <v>6</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B77" s="10">
         <v>43</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C77" s="10">
         <v>43</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D77" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+    <row r="78" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="10">
         <v>6</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B78" s="10">
         <v>44</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C78" s="10">
         <v>44</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D78" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+    <row r="79" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="10">
         <v>6</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B79" s="10">
         <v>45</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C79" s="10">
         <v>45</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D79" s="9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+    <row r="80" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="10">
         <v>6</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B80" s="10">
         <v>46</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C80" s="10">
         <v>46</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D80" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+    <row r="81" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="10">
         <v>6</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B81" s="10">
         <v>47</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C81" s="10">
         <v>47</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D81" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
+    <row r="82" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="10">
         <v>6</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B82" s="10">
         <v>48</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C82" s="10">
         <v>48</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D82" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
+    <row r="83" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="10">
         <v>6</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B83" s="10">
         <v>49</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C83" s="10">
         <v>49</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D83" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="5">
+    <row r="84" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="10">
         <v>6</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B84" s="10">
         <v>50</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C84" s="10">
         <v>50</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D84" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="5">
+    <row r="85" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="10">
         <v>6</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B85" s="10">
         <v>78</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D85" s="9" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="5">
+    <row r="86" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="10">
         <v>6</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B86" s="10">
         <v>79</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D86" s="9" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="5">
+    <row r="87" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="10">
         <v>6</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B87" s="10">
         <v>80</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D87" s="9" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="5">
+    <row r="88" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="10">
         <v>7</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B88" s="10">
         <v>51</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C88" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D88" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="5">
+    <row r="89" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="10">
         <v>7</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B89" s="10">
         <v>52</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C89" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D89" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5">
+    <row r="90" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="10">
         <v>7</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B90" s="10">
         <v>53</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C90" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D90" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="5">
+    <row r="91" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="10">
         <v>7</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B91" s="10">
         <v>54</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C91" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D91" s="9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="5">
+    <row r="92" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="10">
         <v>7</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B92" s="10">
         <v>55</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C92" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D92" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="5">
+    <row r="93" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="10">
         <v>7</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B93" s="10">
         <v>56</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C93" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D93" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5">
+    <row r="94" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="10">
         <v>7</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B94" s="10">
         <v>57</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C94" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D94" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="5">
+    <row r="95" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="10">
         <v>7</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B95" s="10">
         <v>58</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C95" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D95" s="9" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="5">
+    <row r="96" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="10">
         <v>7</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B96" s="10">
         <v>59</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C96" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D96" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5">
+    <row r="97" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="10">
         <v>7</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B97" s="10">
         <v>60</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C97" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D97" s="9" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="5">
+    <row r="98" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="10">
         <v>7</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B98" s="10">
         <v>61</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C98" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D98" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="5">
+    <row r="99" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="10">
         <v>7</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B99" s="10">
         <v>62</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C99" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D99" s="9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="5">
-        <v>8</v>
-      </c>
-      <c r="B67" s="5">
-        <v>2</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5">
-        <v>8</v>
-      </c>
-      <c r="B68" s="5">
-        <v>3</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="5">
-        <v>8</v>
-      </c>
-      <c r="B69" s="5">
-        <v>4</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="5">
-        <v>8</v>
-      </c>
-      <c r="B70" s="5">
-        <v>5</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="5">
-        <v>8</v>
-      </c>
-      <c r="B71" s="5">
-        <v>9</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="5">
-        <v>8</v>
-      </c>
-      <c r="B72" s="5">
-        <v>20</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="5">
-        <v>8</v>
-      </c>
-      <c r="B73" s="5">
-        <v>63</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="5">
-        <v>8</v>
-      </c>
-      <c r="B74" s="5">
-        <v>64</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="5">
-        <v>8</v>
-      </c>
-      <c r="B75" s="5">
-        <v>65</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="5">
-        <v>9</v>
-      </c>
-      <c r="B76" s="5">
-        <v>10</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
-        <v>9</v>
-      </c>
-      <c r="B77" s="5">
-        <v>13</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="5">
-        <v>9</v>
-      </c>
-      <c r="B78" s="5">
-        <v>18</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="5">
-        <v>9</v>
-      </c>
-      <c r="B79" s="5">
-        <v>66</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="5">
-        <v>10</v>
-      </c>
-      <c r="B80" s="5">
-        <v>67</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="5">
-        <v>10</v>
-      </c>
-      <c r="B81" s="5">
-        <v>68</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="5">
-        <v>10</v>
-      </c>
-      <c r="B82" s="5">
-        <v>69</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="5">
-        <v>10</v>
-      </c>
-      <c r="B83" s="5">
-        <v>70</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="5">
-        <v>10</v>
-      </c>
-      <c r="B84" s="5">
-        <v>71</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="5">
-        <v>10</v>
-      </c>
-      <c r="B85" s="5">
-        <v>72</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="5">
-        <v>10</v>
-      </c>
-      <c r="B86" s="5">
-        <v>81</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="5">
-        <v>11</v>
-      </c>
-      <c r="B87" s="5">
-        <v>29</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="5">
-        <v>11</v>
-      </c>
-      <c r="B88" s="5">
-        <v>30</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="5">
-        <v>11</v>
-      </c>
-      <c r="B89" s="5">
-        <v>31</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="5">
-        <v>12</v>
-      </c>
-      <c r="B90" s="5">
-        <v>32</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="5">
-        <v>12</v>
-      </c>
-      <c r="B91" s="5">
-        <v>33</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="5">
-        <v>12</v>
-      </c>
-      <c r="B92" s="5">
-        <v>39</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="5">
-        <v>12</v>
-      </c>
-      <c r="B93" s="5">
-        <v>40</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="5">
-        <v>12</v>
-      </c>
-      <c r="B94" s="5">
-        <v>73</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="5">
-        <v>12</v>
-      </c>
-      <c r="B95" s="5">
-        <v>74</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="5">
-        <v>12</v>
-      </c>
-      <c r="B96" s="5">
-        <v>75</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="5">
-        <v>12</v>
-      </c>
-      <c r="B97" s="5">
-        <v>82</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="5">
-        <v>13</v>
-      </c>
-      <c r="B98" s="5">
-        <v>76</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="5">
-        <v>13</v>
-      </c>
-      <c r="B99" s="5">
-        <v>77</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D99" xr:uid="{DE6C8E3C-CACE-43DC-8D6E-9E79AA11982A}">
-    <sortState ref="A2:D99">
-      <sortCondition ref="A1:A99"/>
+  <autoFilter ref="A1:D74" xr:uid="{DE6C8E3C-CACE-43DC-8D6E-9E79AA11982A}">
+    <sortState ref="A2:D74">
+      <sortCondition ref="A1:A74"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:D99">
-    <sortCondition ref="B2:B99"/>
+  <sortState ref="A2:D74">
+    <sortCondition ref="B2:B74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CANS-56. Updated the Annotated Cans excel file to comply with the items order
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank_2018-06-17.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank_2018-06-17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metquota/cwds/cans-api/tools/instrument-parser/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E6E9504D-FB31-014E-B29F-E40F95A91968}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{62FD536E-780E-6F43-9593-E0FB63759F08}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1980" windowWidth="29960" windowHeight="18320" tabRatio="555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16680" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="4" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Domain_Items" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Domain_Items!$A$1:$D$74</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$A$1:$W$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Domain_Items!$A$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$A$1:$X$83</definedName>
     <definedName name="_Toc328064535" localSheetId="1">Items!$I$3</definedName>
     <definedName name="_Toc513575314" localSheetId="0">Domains!$B$4</definedName>
   </definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="780">
   <si>
     <t>Domain_ID</t>
   </si>
@@ -3135,12 +3135,15 @@
   <si>
     <t>CAREGIVER_EMOTIONAL_RESPONSIVENESS</t>
   </si>
+  <si>
+    <t>Confidential_by_Default</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3546,10 +3549,10 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -3559,7 +3562,7 @@
     <col min="6" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3638,7 +3641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3673,7 +3676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3708,7 +3711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3743,7 +3746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3778,7 +3781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3848,7 +3851,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3906,7 +3909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3935,7 +3938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3964,7 +3967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3993,7 +3996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -4029,15 +4032,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W83"/>
+  <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="27" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="2" hidden="1" customWidth="1"/>
@@ -4046,19 +4049,19 @@
     <col min="5" max="5" width="28.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="32.5" style="2" customWidth="1"/>
     <col min="7" max="12" width="7.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="93.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="7.6640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.83203125" style="2"/>
+    <col min="13" max="14" width="7.6640625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="93.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="7.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="27" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>410</v>
       </c>
@@ -4098,38 +4101,41 @@
       <c r="M1" s="9" t="s">
         <v>775</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="27" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4157,20 +4163,20 @@
       <c r="J2" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="27" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4201,23 +4207,23 @@
       <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="2">
-        <v>1</v>
-      </c>
       <c r="Q3" s="2">
         <v>1</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
       </c>
-      <c r="U3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="27" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4248,23 +4254,23 @@
       <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="2">
-        <v>1</v>
-      </c>
       <c r="Q4" s="2">
         <v>1</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
       </c>
-      <c r="U4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="27" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4295,23 +4301,23 @@
       <c r="J5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="2">
-        <v>1</v>
-      </c>
       <c r="Q5" s="2">
         <v>1</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
       </c>
-      <c r="U5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="27" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4342,23 +4348,23 @@
       <c r="J6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="2">
-        <v>1</v>
-      </c>
       <c r="Q6" s="2">
         <v>1</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
       </c>
-      <c r="U6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="2">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="27" customHeight="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4386,20 +4392,20 @@
       <c r="J7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="2">
-        <v>1</v>
-      </c>
       <c r="R7" s="2">
         <v>1</v>
       </c>
-      <c r="U7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="27" customHeight="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4427,23 +4433,26 @@
       <c r="J8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" s="9">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="2">
-        <v>1</v>
-      </c>
       <c r="R8" s="2">
         <v>1</v>
       </c>
-      <c r="U8" s="2">
+      <c r="S8" s="2">
         <v>1</v>
       </c>
       <c r="V8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="27" customHeight="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4471,20 +4480,20 @@
       <c r="J9" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="Q9" s="2">
-        <v>1</v>
-      </c>
       <c r="R9" s="2">
         <v>1</v>
       </c>
-      <c r="U9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="2">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="27" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4515,23 +4524,23 @@
       <c r="J10" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P10" s="2">
-        <v>1</v>
-      </c>
       <c r="Q10" s="2">
         <v>1</v>
       </c>
       <c r="R10" s="2">
         <v>1</v>
       </c>
-      <c r="U10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S10" s="2">
+        <v>1</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="27" customHeight="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4562,23 +4571,23 @@
       <c r="J11" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="P11" s="2">
-        <v>1</v>
-      </c>
       <c r="Q11" s="2">
         <v>1</v>
       </c>
       <c r="R11" s="2">
         <v>1</v>
       </c>
-      <c r="U11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S11" s="2">
+        <v>1</v>
+      </c>
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="27" customHeight="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -4606,20 +4615,20 @@
       <c r="J12" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="Q12" s="2">
-        <v>1</v>
-      </c>
       <c r="R12" s="2">
         <v>1</v>
       </c>
-      <c r="U12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S12" s="2">
+        <v>1</v>
+      </c>
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="27" customHeight="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -4647,20 +4656,20 @@
       <c r="J13" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="Q13" s="2">
-        <v>1</v>
-      </c>
       <c r="R13" s="2">
         <v>1</v>
       </c>
-      <c r="U13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S13" s="2">
+        <v>1</v>
+      </c>
+      <c r="V13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="27" customHeight="1">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -4691,23 +4700,23 @@
       <c r="J14" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="P14" s="2">
-        <v>1</v>
-      </c>
       <c r="Q14" s="2">
         <v>1</v>
       </c>
       <c r="R14" s="2">
         <v>1</v>
       </c>
-      <c r="U14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" s="2">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="27" customHeight="1">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4735,20 +4744,20 @@
       <c r="J15" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="Q15" s="2">
-        <v>1</v>
-      </c>
       <c r="R15" s="2">
         <v>1</v>
       </c>
-      <c r="U15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S15" s="2">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="27" customHeight="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4776,20 +4785,20 @@
       <c r="J16" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="Q16" s="2">
-        <v>1</v>
-      </c>
       <c r="R16" s="2">
         <v>1</v>
       </c>
-      <c r="U16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S16" s="2">
+        <v>1</v>
+      </c>
+      <c r="V16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="27" customHeight="1">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4817,20 +4826,20 @@
       <c r="J17" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="Q17" s="2">
-        <v>1</v>
-      </c>
       <c r="R17" s="2">
         <v>1</v>
       </c>
-      <c r="U17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S17" s="2">
+        <v>1</v>
+      </c>
+      <c r="V17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="27" customHeight="1">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -4858,20 +4867,20 @@
       <c r="J18" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="Q18" s="2">
-        <v>1</v>
-      </c>
       <c r="R18" s="2">
         <v>1</v>
       </c>
-      <c r="U18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S18" s="2">
+        <v>1</v>
+      </c>
+      <c r="V18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="27" customHeight="1">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4902,20 +4911,20 @@
       <c r="J19" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="Q19" s="2">
-        <v>1</v>
-      </c>
       <c r="R19" s="2">
         <v>1</v>
       </c>
-      <c r="U19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S19" s="2">
+        <v>1</v>
+      </c>
+      <c r="V19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="27" customHeight="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4943,20 +4952,20 @@
       <c r="J20" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="O20" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="Q20" s="2">
-        <v>1</v>
-      </c>
       <c r="R20" s="2">
         <v>1</v>
       </c>
-      <c r="U20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S20" s="2">
+        <v>1</v>
+      </c>
+      <c r="V20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="27" customHeight="1">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4990,23 +4999,23 @@
       <c r="M21" s="9">
         <v>1</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="O21" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="P21" s="2">
-        <v>1</v>
-      </c>
       <c r="Q21" s="2">
         <v>1</v>
       </c>
       <c r="R21" s="2">
         <v>1</v>
       </c>
-      <c r="U21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S21" s="2">
+        <v>1</v>
+      </c>
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="27" customHeight="1">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -5034,23 +5043,23 @@
       <c r="J22" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="Q22" s="2">
-        <v>1</v>
-      </c>
       <c r="R22" s="2">
         <v>1</v>
       </c>
-      <c r="U22" s="2">
+      <c r="S22" s="2">
         <v>1</v>
       </c>
       <c r="V22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="27" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -5078,23 +5087,23 @@
       <c r="J23" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="O23" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="Q23" s="2">
-        <v>1</v>
-      </c>
       <c r="R23" s="2">
         <v>1</v>
       </c>
-      <c r="U23" s="2">
+      <c r="S23" s="2">
         <v>1</v>
       </c>
       <c r="V23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="27" customHeight="1">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -5122,23 +5131,23 @@
       <c r="J24" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="Q24" s="2">
-        <v>1</v>
-      </c>
       <c r="R24" s="2">
         <v>1</v>
       </c>
-      <c r="U24" s="2">
+      <c r="S24" s="2">
         <v>1</v>
       </c>
       <c r="V24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="27" customHeight="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -5166,23 +5175,23 @@
       <c r="J25" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="O25" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="Q25" s="2">
-        <v>1</v>
-      </c>
       <c r="R25" s="2">
         <v>1</v>
       </c>
-      <c r="U25" s="2">
-        <v>1</v>
-      </c>
-      <c r="W25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S25" s="2">
+        <v>1</v>
+      </c>
+      <c r="V25" s="2">
+        <v>1</v>
+      </c>
+      <c r="X25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="27" customHeight="1">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -5210,23 +5219,23 @@
       <c r="J26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="Q26" s="2">
-        <v>1</v>
-      </c>
       <c r="R26" s="2">
         <v>1</v>
       </c>
-      <c r="U26" s="2">
+      <c r="S26" s="2">
         <v>1</v>
       </c>
       <c r="V26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="27" customHeight="1">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -5254,23 +5263,23 @@
       <c r="J27" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="Q27" s="2">
-        <v>1</v>
-      </c>
       <c r="R27" s="2">
         <v>1</v>
       </c>
-      <c r="U27" s="2">
-        <v>1</v>
-      </c>
-      <c r="W27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S27" s="2">
+        <v>1</v>
+      </c>
+      <c r="V27" s="2">
+        <v>1</v>
+      </c>
+      <c r="X27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="27" customHeight="1">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -5298,16 +5307,13 @@
       <c r="J28" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="O28" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="Q28" s="2">
-        <v>1</v>
-      </c>
       <c r="R28" s="2">
         <v>1</v>
       </c>
-      <c r="U28" s="2">
+      <c r="S28" s="2">
         <v>1</v>
       </c>
       <c r="V28" s="2">
@@ -5316,8 +5322,11 @@
       <c r="W28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="27" customHeight="1">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5345,20 +5354,20 @@
       <c r="J29" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="Q29" s="2">
-        <v>1</v>
-      </c>
       <c r="R29" s="2">
         <v>1</v>
       </c>
-      <c r="U29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S29" s="2">
+        <v>1</v>
+      </c>
+      <c r="V29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="27" customHeight="1">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5389,23 +5398,23 @@
       <c r="J30" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="P30" s="2">
-        <v>1</v>
-      </c>
       <c r="Q30" s="2">
         <v>1</v>
       </c>
       <c r="R30" s="2">
         <v>1</v>
       </c>
-      <c r="U30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S30" s="2">
+        <v>1</v>
+      </c>
+      <c r="V30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="27" customHeight="1">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5436,23 +5445,23 @@
       <c r="J31" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="O31" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="P31" s="2">
-        <v>1</v>
-      </c>
       <c r="Q31" s="2">
         <v>1</v>
       </c>
       <c r="R31" s="2">
         <v>1</v>
       </c>
-      <c r="U31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S31" s="2">
+        <v>1</v>
+      </c>
+      <c r="V31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="27" customHeight="1">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5483,23 +5492,23 @@
       <c r="J32" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="O32" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="P32" s="2">
-        <v>1</v>
-      </c>
       <c r="Q32" s="2">
         <v>1</v>
       </c>
       <c r="R32" s="2">
         <v>1</v>
       </c>
-      <c r="U32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S32" s="2">
+        <v>1</v>
+      </c>
+      <c r="V32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="27" customHeight="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5530,23 +5539,23 @@
       <c r="J33" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="N33" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="P33" s="2">
-        <v>1</v>
-      </c>
       <c r="Q33" s="2">
         <v>1</v>
       </c>
-      <c r="S33" s="2">
-        <v>1</v>
-      </c>
-      <c r="U33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R33" s="2">
+        <v>1</v>
+      </c>
+      <c r="T33" s="2">
+        <v>1</v>
+      </c>
+      <c r="V33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="27" customHeight="1">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5577,26 +5586,26 @@
       <c r="J34" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="P34" s="2">
-        <v>1</v>
-      </c>
       <c r="Q34" s="2">
         <v>1</v>
       </c>
-      <c r="S34" s="2">
-        <v>1</v>
-      </c>
-      <c r="U34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R34" s="2">
+        <v>1</v>
+      </c>
+      <c r="T34" s="2">
+        <v>1</v>
+      </c>
+      <c r="V34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="27" customHeight="1">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5627,20 +5636,20 @@
       <c r="M35" s="9">
         <v>1</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="O35" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="Q35" s="2">
-        <v>1</v>
-      </c>
-      <c r="S35" s="2">
-        <v>1</v>
-      </c>
-      <c r="U35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R35" s="2">
+        <v>1</v>
+      </c>
+      <c r="T35" s="2">
+        <v>1</v>
+      </c>
+      <c r="V35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="27" customHeight="1">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5668,20 +5677,20 @@
       <c r="J36" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="Q36" s="2">
-        <v>1</v>
-      </c>
-      <c r="S36" s="2">
-        <v>1</v>
-      </c>
-      <c r="U36" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R36" s="2">
+        <v>1</v>
+      </c>
+      <c r="T36" s="2">
+        <v>1</v>
+      </c>
+      <c r="V36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="27" customHeight="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5709,20 +5718,20 @@
       <c r="J37" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="O37" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="Q37" s="2">
-        <v>1</v>
-      </c>
-      <c r="S37" s="2">
-        <v>1</v>
-      </c>
-      <c r="U37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R37" s="2">
+        <v>1</v>
+      </c>
+      <c r="T37" s="2">
+        <v>1</v>
+      </c>
+      <c r="V37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="27" customHeight="1">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5750,20 +5759,20 @@
       <c r="J38" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="Q38" s="2">
-        <v>1</v>
-      </c>
-      <c r="S38" s="2">
-        <v>1</v>
-      </c>
-      <c r="U38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R38" s="2">
+        <v>1</v>
+      </c>
+      <c r="T38" s="2">
+        <v>1</v>
+      </c>
+      <c r="V38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="27" customHeight="1">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5791,20 +5800,20 @@
       <c r="J39" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="Q39" s="2">
-        <v>1</v>
-      </c>
-      <c r="S39" s="2">
-        <v>1</v>
-      </c>
-      <c r="U39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R39" s="2">
+        <v>1</v>
+      </c>
+      <c r="T39" s="2">
+        <v>1</v>
+      </c>
+      <c r="V39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="27" customHeight="1">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5835,20 +5844,20 @@
       <c r="J40" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="O40" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="Q40" s="2">
-        <v>1</v>
-      </c>
-      <c r="S40" s="2">
-        <v>1</v>
-      </c>
-      <c r="U40" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R40" s="2">
+        <v>1</v>
+      </c>
+      <c r="T40" s="2">
+        <v>1</v>
+      </c>
+      <c r="V40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="27" customHeight="1">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5879,23 +5888,23 @@
       <c r="J41" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="N41" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="P41" s="2">
-        <v>1</v>
-      </c>
       <c r="Q41" s="2">
         <v>1</v>
       </c>
-      <c r="S41" s="2">
-        <v>1</v>
-      </c>
-      <c r="U41" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R41" s="2">
+        <v>1</v>
+      </c>
+      <c r="T41" s="2">
+        <v>1</v>
+      </c>
+      <c r="V41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="27" customHeight="1">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -5926,23 +5935,23 @@
       <c r="J42" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="P42" s="2">
-        <v>1</v>
-      </c>
       <c r="Q42" s="2">
         <v>1</v>
       </c>
       <c r="R42" s="2">
         <v>1</v>
       </c>
-      <c r="U42" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S42" s="2">
+        <v>1</v>
+      </c>
+      <c r="V42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="27" customHeight="1">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5973,23 +5982,23 @@
       <c r="J43" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="P43" s="2">
-        <v>1</v>
-      </c>
       <c r="Q43" s="2">
         <v>1</v>
       </c>
       <c r="R43" s="2">
         <v>1</v>
       </c>
-      <c r="U43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S43" s="2">
+        <v>1</v>
+      </c>
+      <c r="V43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="27" customHeight="1">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -6020,26 +6029,26 @@
       <c r="J44" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="O44" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="O44" s="2" t="s">
+      <c r="P44" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="P44" s="2">
-        <v>1</v>
-      </c>
       <c r="Q44" s="2">
         <v>1</v>
       </c>
       <c r="R44" s="2">
         <v>1</v>
       </c>
-      <c r="U44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S44" s="2">
+        <v>1</v>
+      </c>
+      <c r="V44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="27" customHeight="1">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -6070,23 +6079,23 @@
       <c r="J45" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="P45" s="2">
-        <v>1</v>
-      </c>
       <c r="Q45" s="2">
         <v>1</v>
       </c>
       <c r="R45" s="2">
         <v>1</v>
       </c>
-      <c r="U45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S45" s="2">
+        <v>1</v>
+      </c>
+      <c r="V45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="27" customHeight="1">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -6117,23 +6126,23 @@
       <c r="J46" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="P46" s="2">
-        <v>1</v>
-      </c>
       <c r="Q46" s="2">
         <v>1</v>
       </c>
       <c r="R46" s="2">
         <v>1</v>
       </c>
-      <c r="U46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S46" s="2">
+        <v>1</v>
+      </c>
+      <c r="V46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="27" customHeight="1">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -6164,23 +6173,23 @@
       <c r="J47" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="P47" s="2">
-        <v>1</v>
-      </c>
       <c r="Q47" s="2">
         <v>1</v>
       </c>
       <c r="R47" s="2">
         <v>1</v>
       </c>
-      <c r="U47" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S47" s="2">
+        <v>1</v>
+      </c>
+      <c r="V47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="27" customHeight="1">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -6211,23 +6220,23 @@
       <c r="J48" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="N48" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="P48" s="2">
-        <v>1</v>
-      </c>
       <c r="Q48" s="2">
         <v>1</v>
       </c>
       <c r="R48" s="2">
         <v>1</v>
       </c>
-      <c r="U48" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S48" s="2">
+        <v>1</v>
+      </c>
+      <c r="V48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="27" customHeight="1">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -6258,26 +6267,29 @@
       <c r="J49" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="N49" s="9">
+        <v>1</v>
+      </c>
+      <c r="O49" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="P49" s="2">
-        <v>1</v>
-      </c>
       <c r="Q49" s="2">
         <v>1</v>
       </c>
       <c r="R49" s="2">
         <v>1</v>
       </c>
-      <c r="U49" s="2">
+      <c r="S49" s="2">
         <v>1</v>
       </c>
       <c r="V49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="27" customHeight="1">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -6308,23 +6320,23 @@
       <c r="J50" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="N50" s="2" t="s">
+      <c r="O50" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="P50" s="2">
-        <v>1</v>
-      </c>
       <c r="Q50" s="2">
         <v>1</v>
       </c>
       <c r="R50" s="2">
         <v>1</v>
       </c>
-      <c r="U50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S50" s="2">
+        <v>1</v>
+      </c>
+      <c r="V50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" ht="27" customHeight="1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -6355,23 +6367,23 @@
       <c r="J51" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="N51" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="P51" s="2">
-        <v>1</v>
-      </c>
       <c r="Q51" s="2">
         <v>1</v>
       </c>
       <c r="R51" s="2">
         <v>1</v>
       </c>
-      <c r="U51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S51" s="2">
+        <v>1</v>
+      </c>
+      <c r="V51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="27" customHeight="1">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -6396,23 +6408,23 @@
       <c r="L52" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="N52" s="2" t="s">
+      <c r="O52" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="P52" s="2">
-        <v>1</v>
-      </c>
       <c r="Q52" s="2">
         <v>1</v>
       </c>
       <c r="R52" s="2">
         <v>1</v>
       </c>
-      <c r="T52" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S52" s="2">
+        <v>1</v>
+      </c>
+      <c r="U52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="27" customHeight="1">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -6437,23 +6449,23 @@
       <c r="L53" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="N53" s="2" t="s">
+      <c r="O53" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="P53" s="2">
-        <v>1</v>
-      </c>
       <c r="Q53" s="2">
         <v>1</v>
       </c>
       <c r="R53" s="2">
         <v>1</v>
       </c>
-      <c r="T53" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S53" s="2">
+        <v>1</v>
+      </c>
+      <c r="U53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="27" customHeight="1">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -6478,23 +6490,23 @@
       <c r="L54" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="N54" s="2" t="s">
+      <c r="O54" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="P54" s="2">
-        <v>1</v>
-      </c>
       <c r="Q54" s="2">
         <v>1</v>
       </c>
       <c r="R54" s="2">
         <v>1</v>
       </c>
-      <c r="T54" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S54" s="2">
+        <v>1</v>
+      </c>
+      <c r="U54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="27" customHeight="1">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -6519,23 +6531,23 @@
       <c r="L55" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N55" s="2" t="s">
+      <c r="O55" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="P55" s="2">
-        <v>1</v>
-      </c>
       <c r="Q55" s="2">
         <v>1</v>
       </c>
       <c r="R55" s="2">
         <v>1</v>
       </c>
-      <c r="T55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S55" s="2">
+        <v>1</v>
+      </c>
+      <c r="U55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="27" customHeight="1">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -6560,26 +6572,26 @@
       <c r="L56" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="N56" s="2" t="s">
+      <c r="O56" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="O56" s="2" t="s">
+      <c r="P56" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="P56" s="2">
-        <v>1</v>
-      </c>
       <c r="Q56" s="2">
         <v>1</v>
       </c>
       <c r="R56" s="2">
         <v>1</v>
       </c>
-      <c r="T56" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S56" s="2">
+        <v>1</v>
+      </c>
+      <c r="U56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="27" customHeight="1">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -6604,23 +6616,23 @@
       <c r="L57" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="N57" s="2" t="s">
+      <c r="O57" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="P57" s="2">
-        <v>1</v>
-      </c>
       <c r="Q57" s="2">
         <v>1</v>
       </c>
       <c r="R57" s="2">
         <v>1</v>
       </c>
-      <c r="T57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S57" s="2">
+        <v>1</v>
+      </c>
+      <c r="U57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="27" customHeight="1">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -6645,23 +6657,23 @@
       <c r="L58" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="N58" s="2" t="s">
+      <c r="O58" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="P58" s="2">
-        <v>1</v>
-      </c>
       <c r="Q58" s="2">
         <v>1</v>
       </c>
       <c r="R58" s="2">
         <v>1</v>
       </c>
-      <c r="T58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S58" s="2">
+        <v>1</v>
+      </c>
+      <c r="U58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="27" customHeight="1">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -6686,23 +6698,23 @@
       <c r="L59" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="N59" s="2" t="s">
+      <c r="O59" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="P59" s="2">
-        <v>1</v>
-      </c>
       <c r="Q59" s="2">
         <v>1</v>
       </c>
       <c r="R59" s="2">
         <v>1</v>
       </c>
-      <c r="T59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S59" s="2">
+        <v>1</v>
+      </c>
+      <c r="U59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" ht="27" customHeight="1">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -6727,26 +6739,26 @@
       <c r="L60" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="N60" s="2" t="s">
+      <c r="O60" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="O60" s="2" t="s">
+      <c r="P60" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="P60" s="2">
-        <v>1</v>
-      </c>
       <c r="Q60" s="2">
         <v>1</v>
       </c>
       <c r="R60" s="2">
         <v>1</v>
       </c>
-      <c r="T60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S60" s="2">
+        <v>1</v>
+      </c>
+      <c r="U60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="27" customHeight="1">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -6771,26 +6783,26 @@
       <c r="L61" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="N61" s="2" t="s">
+      <c r="O61" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="O61" s="2" t="s">
+      <c r="P61" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="P61" s="2">
-        <v>1</v>
-      </c>
       <c r="Q61" s="2">
         <v>1</v>
       </c>
       <c r="R61" s="2">
         <v>1</v>
       </c>
-      <c r="T61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S61" s="2">
+        <v>1</v>
+      </c>
+      <c r="U61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="27" customHeight="1">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -6815,26 +6827,26 @@
       <c r="L62" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="N62" s="2" t="s">
+      <c r="O62" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="O62" s="2" t="s">
+      <c r="P62" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="P62" s="2">
-        <v>1</v>
-      </c>
       <c r="Q62" s="2">
         <v>1</v>
       </c>
       <c r="R62" s="2">
         <v>1</v>
       </c>
-      <c r="T62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S62" s="2">
+        <v>1</v>
+      </c>
+      <c r="U62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="27" customHeight="1">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -6859,23 +6871,23 @@
       <c r="L63" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="N63" s="2" t="s">
+      <c r="O63" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="P63" s="2">
-        <v>1</v>
-      </c>
       <c r="Q63" s="2">
         <v>1</v>
       </c>
       <c r="R63" s="2">
         <v>1</v>
       </c>
-      <c r="T63" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S63" s="2">
+        <v>1</v>
+      </c>
+      <c r="U63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="27" customHeight="1">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -6903,23 +6915,23 @@
       <c r="J64" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="N64" s="2" t="s">
+      <c r="O64" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="P64" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q64" s="2" t="s">
+      <c r="Q64" s="2">
+        <v>1</v>
+      </c>
+      <c r="R64" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R64" s="2">
-        <v>1</v>
-      </c>
-      <c r="U64" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S64" s="2">
+        <v>1</v>
+      </c>
+      <c r="V64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" ht="27" customHeight="1">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -6947,23 +6959,23 @@
       <c r="J65" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="N65" s="2" t="s">
+      <c r="O65" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="P65" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="2" t="s">
+      <c r="Q65" s="2">
+        <v>1</v>
+      </c>
+      <c r="R65" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R65" s="2">
-        <v>1</v>
-      </c>
-      <c r="U65" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S65" s="2">
+        <v>1</v>
+      </c>
+      <c r="V65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" ht="27" customHeight="1">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -6991,23 +7003,23 @@
       <c r="J66" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="N66" s="2" t="s">
+      <c r="O66" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="P66" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q66" s="2" t="s">
+      <c r="Q66" s="2">
+        <v>1</v>
+      </c>
+      <c r="R66" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R66" s="2">
-        <v>1</v>
-      </c>
-      <c r="U66" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S66" s="2">
+        <v>1</v>
+      </c>
+      <c r="V66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" ht="27" customHeight="1">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -7035,23 +7047,23 @@
       <c r="J67" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="N67" s="2" t="s">
+      <c r="O67" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="P67" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="2" t="s">
+      <c r="Q67" s="2">
+        <v>1</v>
+      </c>
+      <c r="R67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R67" s="2">
-        <v>1</v>
-      </c>
-      <c r="U67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S67" s="2">
+        <v>1</v>
+      </c>
+      <c r="V67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" ht="27" customHeight="1">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -7079,23 +7091,23 @@
       <c r="J68" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="N68" s="2" t="s">
+      <c r="O68" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="P68" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="2" t="s">
+      <c r="Q68" s="2">
+        <v>1</v>
+      </c>
+      <c r="R68" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R68" s="2">
-        <v>1</v>
-      </c>
-      <c r="U68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S68" s="2">
+        <v>1</v>
+      </c>
+      <c r="V68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="27" customHeight="1">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -7123,26 +7135,26 @@
       <c r="J69" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="N69" s="2" t="s">
+      <c r="O69" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="P69" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q69" s="2" t="s">
+      <c r="Q69" s="2">
+        <v>1</v>
+      </c>
+      <c r="R69" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R69" s="2">
-        <v>1</v>
-      </c>
-      <c r="T69" s="2">
+      <c r="S69" s="2">
         <v>1</v>
       </c>
       <c r="U69" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="27" customHeight="1">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -7170,26 +7182,26 @@
       <c r="J70" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="N70" s="2" t="s">
+      <c r="O70" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="P70" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q70" s="2" t="s">
+      <c r="Q70" s="2">
+        <v>1</v>
+      </c>
+      <c r="R70" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R70" s="2">
-        <v>1</v>
-      </c>
-      <c r="T70" s="2">
+      <c r="S70" s="2">
         <v>1</v>
       </c>
       <c r="U70" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" ht="27" customHeight="1">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -7217,26 +7229,29 @@
       <c r="J71" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="N71" s="2" t="s">
+      <c r="N71" s="9">
+        <v>1</v>
+      </c>
+      <c r="O71" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="P71" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q71" s="2" t="s">
+      <c r="Q71" s="2">
+        <v>1</v>
+      </c>
+      <c r="R71" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R71" s="2">
-        <v>1</v>
-      </c>
-      <c r="T71" s="2">
+      <c r="S71" s="2">
         <v>1</v>
       </c>
       <c r="U71" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" ht="27" customHeight="1">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -7264,26 +7279,26 @@
       <c r="J72" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="N72" s="2" t="s">
+      <c r="O72" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="P72" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q72" s="2" t="s">
+      <c r="Q72" s="2">
+        <v>1</v>
+      </c>
+      <c r="R72" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R72" s="2">
-        <v>1</v>
-      </c>
-      <c r="T72" s="2">
+      <c r="S72" s="2">
         <v>1</v>
       </c>
       <c r="U72" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="27" customHeight="1">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -7311,26 +7326,26 @@
       <c r="J73" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="N73" s="2" t="s">
+      <c r="O73" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="P73" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="2" t="s">
+      <c r="Q73" s="2">
+        <v>1</v>
+      </c>
+      <c r="R73" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R73" s="2">
-        <v>1</v>
-      </c>
-      <c r="T73" s="2">
+      <c r="S73" s="2">
         <v>1</v>
       </c>
       <c r="U73" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="27" customHeight="1">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -7358,26 +7373,26 @@
       <c r="J74" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="N74" s="2" t="s">
+      <c r="O74" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="P74" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q74" s="2" t="s">
+      <c r="Q74" s="2">
+        <v>1</v>
+      </c>
+      <c r="R74" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R74" s="2">
-        <v>1</v>
-      </c>
-      <c r="T74" s="2">
+      <c r="S74" s="2">
         <v>1</v>
       </c>
       <c r="U74" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" ht="27" customHeight="1">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -7405,26 +7420,26 @@
       <c r="J75" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="N75" s="2" t="s">
+      <c r="O75" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="P75" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q75" s="2" t="s">
+      <c r="Q75" s="2">
+        <v>1</v>
+      </c>
+      <c r="R75" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R75" s="2">
-        <v>1</v>
-      </c>
-      <c r="T75" s="2">
+      <c r="S75" s="2">
         <v>1</v>
       </c>
       <c r="U75" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" ht="27" customHeight="1">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -7452,23 +7467,23 @@
       <c r="J76" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="N76" s="2" t="s">
+      <c r="O76" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="P76" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q76" s="2" t="s">
+      <c r="Q76" s="2">
+        <v>1</v>
+      </c>
+      <c r="R76" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R76" s="2">
-        <v>1</v>
-      </c>
-      <c r="U76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S76" s="2">
+        <v>1</v>
+      </c>
+      <c r="V76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" ht="27" customHeight="1">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -7496,23 +7511,23 @@
       <c r="J77" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="N77" s="2" t="s">
+      <c r="O77" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="P77" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q77" s="2" t="s">
+      <c r="Q77" s="2">
+        <v>1</v>
+      </c>
+      <c r="R77" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R77" s="2">
-        <v>1</v>
-      </c>
-      <c r="U77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S77" s="2">
+        <v>1</v>
+      </c>
+      <c r="V77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" ht="27" customHeight="1">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -7540,23 +7555,23 @@
       <c r="J78" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="N78" s="2" t="s">
+      <c r="O78" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="P78" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q78" s="2" t="s">
+      <c r="Q78" s="2">
+        <v>1</v>
+      </c>
+      <c r="R78" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R78" s="2">
-        <v>1</v>
-      </c>
-      <c r="U78" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S78" s="2">
+        <v>1</v>
+      </c>
+      <c r="V78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" ht="27" customHeight="1">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -7584,23 +7599,23 @@
       <c r="J79" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="N79" s="2" t="s">
+      <c r="O79" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="P79" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q79" s="2" t="s">
+      <c r="Q79" s="2">
+        <v>1</v>
+      </c>
+      <c r="R79" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R79" s="2">
-        <v>1</v>
-      </c>
-      <c r="U79" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S79" s="2">
+        <v>1</v>
+      </c>
+      <c r="V79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" ht="27" customHeight="1">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -7628,23 +7643,23 @@
       <c r="J80" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="N80" s="2" t="s">
+      <c r="O80" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="P80" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q80" s="2" t="s">
+      <c r="Q80" s="2">
+        <v>1</v>
+      </c>
+      <c r="R80" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R80" s="2">
-        <v>1</v>
-      </c>
-      <c r="U80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S80" s="2">
+        <v>1</v>
+      </c>
+      <c r="V80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" ht="27" customHeight="1">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -7672,23 +7687,23 @@
       <c r="J81" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="N81" s="2" t="s">
+      <c r="O81" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="P81" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q81" s="2" t="s">
+      <c r="Q81" s="2">
+        <v>1</v>
+      </c>
+      <c r="R81" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R81" s="2">
-        <v>1</v>
-      </c>
-      <c r="U81" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S81" s="2">
+        <v>1</v>
+      </c>
+      <c r="V81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" ht="27" customHeight="1">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -7719,23 +7734,23 @@
       <c r="M82" s="9">
         <v>1</v>
       </c>
-      <c r="N82" s="2" t="s">
+      <c r="O82" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="P82" s="2">
-        <v>1</v>
-      </c>
-      <c r="R82" s="2">
-        <v>1</v>
-      </c>
-      <c r="U82" s="2">
+      <c r="Q82" s="2">
+        <v>1</v>
+      </c>
+      <c r="S82" s="2">
         <v>1</v>
       </c>
       <c r="V82" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" ht="27" customHeight="1">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -7763,23 +7778,23 @@
       <c r="J83" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="N83" s="2" t="s">
+      <c r="O83" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="R83" s="2">
-        <v>1</v>
-      </c>
-      <c r="U83" s="2">
+      <c r="S83" s="2">
+        <v>1</v>
+      </c>
+      <c r="V83" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W83" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState ref="A2:W83">
+  <autoFilter ref="A1:X83" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState ref="A2:X83">
       <sortCondition ref="A1:A83"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A1:W91">
+  <sortState ref="A1:X91">
     <sortCondition ref="C2:C81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7791,11 +7806,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
@@ -7803,7 +7818,7 @@
     <col min="5" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7817,7 +7832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7828,7 +7843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7839,7 +7854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -7850,7 +7865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -7861,7 +7876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -7872,7 +7887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -7883,7 +7898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -7894,7 +7909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -7905,7 +7920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -7916,7 +7931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -7927,7 +7942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -7938,7 +7953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="5">
         <v>2</v>
       </c>
@@ -7949,7 +7964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="5">
         <v>2</v>
       </c>
@@ -7960,7 +7975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -7971,7 +7986,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -7982,7 +7997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="5">
         <v>2</v>
       </c>
@@ -7993,7 +8008,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="5">
         <v>2</v>
       </c>
@@ -8004,7 +8019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="5">
         <v>2</v>
       </c>
@@ -8015,7 +8030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="5">
         <v>2</v>
       </c>
@@ -8026,7 +8041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -8037,7 +8052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="5">
         <v>3</v>
       </c>
@@ -8048,7 +8063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="5">
         <v>3</v>
       </c>
@@ -8059,7 +8074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="5">
         <v>3</v>
       </c>
@@ -8070,7 +8085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="5">
         <v>3</v>
       </c>
@@ -8081,7 +8096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="5">
         <v>3</v>
       </c>
@@ -8092,7 +8107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="5">
         <v>3</v>
       </c>
@@ -8103,7 +8118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="5">
         <v>3</v>
       </c>
@@ -8114,7 +8129,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" s="5">
         <v>3</v>
       </c>
@@ -8125,7 +8140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" s="5">
         <v>4</v>
       </c>
@@ -8136,7 +8151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" s="5">
         <v>4</v>
       </c>
@@ -8147,7 +8162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" s="5">
         <v>4</v>
       </c>
@@ -8158,7 +8173,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="5">
         <v>5</v>
       </c>
@@ -8169,7 +8184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="5">
         <v>5</v>
       </c>
@@ -8180,7 +8195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="5">
         <v>5</v>
       </c>
@@ -8191,7 +8206,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="5">
         <v>5</v>
       </c>
@@ -8202,7 +8217,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="5">
         <v>5</v>
       </c>
@@ -8213,7 +8228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="5">
         <v>5</v>
       </c>
@@ -8224,7 +8239,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="5">
         <v>5</v>
       </c>
@@ -8235,7 +8250,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="5">
         <v>5</v>
       </c>
@@ -8246,7 +8261,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="5">
         <v>5</v>
       </c>
@@ -8257,370 +8272,370 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="5">
         <v>8</v>
       </c>
       <c r="B42" s="5">
         <v>2</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="5">
         <v>8</v>
       </c>
       <c r="B43" s="5">
         <v>3</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="5">
         <v>8</v>
       </c>
       <c r="B44" s="5">
         <v>4</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="5">
         <v>8</v>
       </c>
       <c r="B45" s="5">
         <v>5</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="5">
         <v>8</v>
       </c>
       <c r="B46" s="5">
         <v>9</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="5">
         <v>8</v>
       </c>
       <c r="B47" s="5">
-        <v>20</v>
-      </c>
-      <c r="D47" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="5">
         <v>8</v>
       </c>
       <c r="B48" s="5">
-        <v>63</v>
-      </c>
-      <c r="D48" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5">
         <v>8</v>
       </c>
       <c r="B49" s="5">
-        <v>64</v>
-      </c>
-      <c r="D49" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="5">
         <v>8</v>
       </c>
       <c r="B50" s="5">
-        <v>65</v>
-      </c>
-      <c r="D50" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="5">
         <v>9</v>
       </c>
       <c r="B51" s="5">
         <v>10</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="5">
         <v>9</v>
       </c>
       <c r="B52" s="5">
-        <v>13</v>
-      </c>
-      <c r="D52" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="5">
         <v>9</v>
       </c>
       <c r="B53" s="5">
-        <v>18</v>
-      </c>
-      <c r="D53" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="5">
         <v>9</v>
       </c>
       <c r="B54" s="5">
-        <v>66</v>
-      </c>
-      <c r="D54" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" s="5">
-        <v>67</v>
-      </c>
-      <c r="D55" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="5">
         <v>10</v>
       </c>
       <c r="B56" s="5">
-        <v>68</v>
-      </c>
-      <c r="D56" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="5">
         <v>10</v>
       </c>
       <c r="B57" s="5">
-        <v>69</v>
-      </c>
-      <c r="D57" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="5">
         <v>10</v>
       </c>
       <c r="B58" s="5">
-        <v>70</v>
-      </c>
-      <c r="D58" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="5">
         <v>10</v>
       </c>
       <c r="B59" s="5">
-        <v>71</v>
-      </c>
-      <c r="D59" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" s="5">
         <v>10</v>
       </c>
       <c r="B60" s="5">
-        <v>72</v>
-      </c>
-      <c r="D60" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" s="5">
         <v>10</v>
       </c>
       <c r="B61" s="5">
-        <v>81</v>
-      </c>
-      <c r="D61" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B62" s="5">
-        <v>29</v>
-      </c>
-      <c r="D62" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="5">
         <v>11</v>
       </c>
       <c r="B63" s="5">
-        <v>30</v>
-      </c>
-      <c r="D63" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="5">
         <v>11</v>
       </c>
       <c r="B64" s="5">
+        <v>30</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="5">
+        <v>11</v>
+      </c>
+      <c r="B65" s="5">
         <v>31</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="5">
-        <v>12</v>
-      </c>
-      <c r="B65" s="5">
-        <v>32</v>
-      </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="5">
         <v>12</v>
       </c>
       <c r="B66" s="5">
-        <v>33</v>
-      </c>
-      <c r="D66" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" s="5">
         <v>12</v>
       </c>
       <c r="B67" s="5">
-        <v>39</v>
-      </c>
-      <c r="D67" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68" s="5">
         <v>12</v>
       </c>
       <c r="B68" s="5">
-        <v>40</v>
-      </c>
-      <c r="D68" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" s="5">
         <v>12</v>
       </c>
       <c r="B69" s="5">
-        <v>73</v>
-      </c>
-      <c r="D69" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" s="5">
         <v>12</v>
       </c>
       <c r="B70" s="5">
         <v>74</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" s="5">
         <v>12</v>
       </c>
       <c r="B71" s="5">
         <v>75</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D71" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" s="5">
         <v>12</v>
       </c>
       <c r="B72" s="5">
         <v>82</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" s="5">
         <v>13</v>
       </c>
       <c r="B73" s="5">
         <v>76</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" s="5">
         <v>13</v>
       </c>
       <c r="B74" s="5">
         <v>77</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D74" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" s="10" customFormat="1">
       <c r="A75" s="10">
         <v>6</v>
       </c>
@@ -8634,7 +8649,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" s="10" customFormat="1">
       <c r="A76" s="10">
         <v>6</v>
       </c>
@@ -8648,7 +8663,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" s="10" customFormat="1">
       <c r="A77" s="10">
         <v>6</v>
       </c>
@@ -8662,7 +8677,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" s="10" customFormat="1">
       <c r="A78" s="10">
         <v>6</v>
       </c>
@@ -8676,7 +8691,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" s="10" customFormat="1">
       <c r="A79" s="10">
         <v>6</v>
       </c>
@@ -8690,7 +8705,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" s="10" customFormat="1">
       <c r="A80" s="10">
         <v>6</v>
       </c>
@@ -8704,7 +8719,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" s="10" customFormat="1">
       <c r="A81" s="10">
         <v>6</v>
       </c>
@@ -8718,7 +8733,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" s="10" customFormat="1">
       <c r="A82" s="10">
         <v>6</v>
       </c>
@@ -8732,7 +8747,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" s="10" customFormat="1">
       <c r="A83" s="10">
         <v>6</v>
       </c>
@@ -8746,7 +8761,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" s="10" customFormat="1">
       <c r="A84" s="10">
         <v>6</v>
       </c>
@@ -8760,7 +8775,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" s="10" customFormat="1">
       <c r="A85" s="10">
         <v>6</v>
       </c>
@@ -8771,7 +8786,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" s="10" customFormat="1">
       <c r="A86" s="10">
         <v>6</v>
       </c>
@@ -8782,7 +8797,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" s="10" customFormat="1">
       <c r="A87" s="10">
         <v>6</v>
       </c>
@@ -8793,7 +8808,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" s="10" customFormat="1">
       <c r="A88" s="10">
         <v>7</v>
       </c>
@@ -8807,7 +8822,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" s="10" customFormat="1">
       <c r="A89" s="10">
         <v>7</v>
       </c>
@@ -8821,7 +8836,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" s="10" customFormat="1">
       <c r="A90" s="10">
         <v>7</v>
       </c>
@@ -8835,7 +8850,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" s="10" customFormat="1">
       <c r="A91" s="10">
         <v>7</v>
       </c>
@@ -8849,7 +8864,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" s="10" customFormat="1">
       <c r="A92" s="10">
         <v>7</v>
       </c>
@@ -8863,7 +8878,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" s="10" customFormat="1">
       <c r="A93" s="10">
         <v>7</v>
       </c>
@@ -8877,7 +8892,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" s="10" customFormat="1">
       <c r="A94" s="10">
         <v>7</v>
       </c>
@@ -8891,7 +8906,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" s="10" customFormat="1">
       <c r="A95" s="10">
         <v>7</v>
       </c>
@@ -8905,7 +8920,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" s="10" customFormat="1">
       <c r="A96" s="10">
         <v>7</v>
       </c>
@@ -8919,7 +8934,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" s="10" customFormat="1">
       <c r="A97" s="10">
         <v>7</v>
       </c>
@@ -8933,7 +8948,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" s="10" customFormat="1">
       <c r="A98" s="10">
         <v>7</v>
       </c>
@@ -8947,7 +8962,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="99" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" s="10" customFormat="1">
       <c r="A99" s="10">
         <v>7</v>
       </c>
@@ -8962,14 +8977,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D74" xr:uid="{DE6C8E3C-CACE-43DC-8D6E-9E79AA11982A}">
-    <sortState ref="A2:D74">
-      <sortCondition ref="A1:A74"/>
+  <autoFilter ref="A1:D41" xr:uid="{DE6C8E3C-CACE-43DC-8D6E-9E79AA11982A}">
+    <sortState ref="A2:D41">
+      <sortCondition ref="A1:A41"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:D74">
-    <sortCondition ref="B2:B74"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>